<commit_message>
chore: update btech-62 sem1,3 sep9
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 62 (btech-62)/3/1.xlsx
+++ b/raw/time_tables/B.Tech 62 (btech-62)/3/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amit.mishra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fileserver2\time table\Time table Odd 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DC9614-5796-4F4E-8D25-A96C25FC3489}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DCADB3-5604-4493-968F-E3ADFAD4125A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1287,9 +1287,6 @@
     <t>LA5-A6(HS211)-CR401/AMN</t>
   </si>
   <si>
-    <t>TB9(HS211)-TS13/KMB</t>
-  </si>
-  <si>
     <t xml:space="preserve">LA10,C3(BT211)-FF2/NV </t>
   </si>
   <si>
@@ -1609,6 +1606,9 @@
   </si>
   <si>
     <t>PB1,B16(B15CS214)-CL05,06/PRK,PKU</t>
+  </si>
+  <si>
+    <t>TB9(HS211)-TS12/KMB</t>
   </si>
 </sst>
 </file>
@@ -2222,38 +2222,67 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2263,15 +2292,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2290,38 +2310,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2550,10 +2550,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47:D47"/>
+      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2575,17 +2575,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="108"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="115"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -2605,7 +2605,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="97" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2651,7 +2651,7 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="56" t="s">
         <v>10</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="E3" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="107" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="56" t="s">
@@ -2697,7 +2697,7 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="56" t="s">
         <v>18</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="E4" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="103"/>
+      <c r="F4" s="108"/>
       <c r="H4" s="56" t="s">
         <v>22</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="56" t="s">
         <v>419</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="E5" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="103"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="56" t="s">
         <v>26</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116"/>
+      <c r="A6" s="98"/>
       <c r="B6" s="56" t="s">
         <v>28</v>
       </c>
@@ -2784,12 +2784,12 @@
         <v>29</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="103"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="57"/>
       <c r="H6" s="56" t="s">
         <v>31</v>
@@ -2816,7 +2816,7 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
+      <c r="A7" s="98"/>
       <c r="B7" s="56" t="s">
         <v>32</v>
       </c>
@@ -2824,12 +2824,12 @@
         <v>399</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="103"/>
+      <c r="F7" s="108"/>
       <c r="G7" s="56" t="s">
         <v>34</v>
       </c>
@@ -2858,7 +2858,7 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="116"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="56" t="s">
         <v>36</v>
       </c>
@@ -2866,12 +2866,12 @@
         <v>37</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E8" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="103"/>
+      <c r="F8" s="108"/>
       <c r="G8" s="56" t="s">
         <v>39</v>
       </c>
@@ -2900,20 +2900,20 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="116"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="58" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D9" s="56" t="s">
         <v>43</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>487</v>
-      </c>
-      <c r="F9" s="103"/>
+        <v>486</v>
+      </c>
+      <c r="F9" s="108"/>
       <c r="G9" s="56" t="s">
         <v>44</v>
       </c>
@@ -2942,9 +2942,9 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="117"/>
+      <c r="A10" s="118"/>
       <c r="B10" s="59" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C10" s="59" t="s">
         <v>47</v>
@@ -2955,7 +2955,7 @@
       <c r="E10" s="86" t="s">
         <v>418</v>
       </c>
-      <c r="F10" s="103"/>
+      <c r="F10" s="108"/>
       <c r="G10" s="56" t="s">
         <v>49</v>
       </c>
@@ -2982,7 +2982,7 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="117"/>
+      <c r="A11" s="118"/>
       <c r="B11" s="59" t="s">
         <v>52</v>
       </c>
@@ -2995,9 +2995,9 @@
       <c r="E11" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="103"/>
+      <c r="F11" s="108"/>
       <c r="G11" s="88" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H11" s="61" t="s">
         <v>73</v>
@@ -3024,7 +3024,7 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
+      <c r="A12" s="118"/>
       <c r="B12" s="62"/>
       <c r="C12" s="59" t="s">
         <v>57</v>
@@ -3035,7 +3035,7 @@
       <c r="E12" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="103"/>
+      <c r="F12" s="108"/>
       <c r="G12" s="56" t="s">
         <v>400</v>
       </c>
@@ -3064,10 +3064,10 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="62"/>
       <c r="C13" s="59" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D13" s="60" t="s">
         <v>62</v>
@@ -3075,7 +3075,7 @@
       <c r="E13" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="103"/>
+      <c r="F13" s="108"/>
       <c r="G13" s="61" t="s">
         <v>64</v>
       </c>
@@ -3102,22 +3102,22 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="118"/>
       <c r="B14" s="59" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>432</v>
-      </c>
-      <c r="F14" s="103"/>
+        <v>431</v>
+      </c>
+      <c r="F14" s="108"/>
       <c r="G14" s="61" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H14" s="63"/>
       <c r="I14" s="56"/>
@@ -3140,7 +3140,7 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="59" t="s">
         <v>68</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="E15" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="103"/>
+      <c r="F15" s="108"/>
       <c r="G15" s="64" t="s">
         <v>72</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
+      <c r="A16" s="118"/>
       <c r="B16" s="59" t="s">
         <v>364</v>
       </c>
@@ -3187,9 +3187,9 @@
         <v>382</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>446</v>
-      </c>
-      <c r="F16" s="120"/>
+        <v>445</v>
+      </c>
+      <c r="F16" s="126"/>
       <c r="G16" s="56" t="s">
         <v>380</v>
       </c>
@@ -3214,19 +3214,19 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
+      <c r="A17" s="118"/>
       <c r="B17" s="87" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C17" s="62"/>
       <c r="E17" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="103"/>
-      <c r="G17" s="121" t="s">
-        <v>439</v>
-      </c>
-      <c r="H17" s="122"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="127" t="s">
+        <v>438</v>
+      </c>
+      <c r="H17" s="128"/>
       <c r="I17" s="56"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -3247,18 +3247,18 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
-      <c r="B18" s="124"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="123" t="s">
+      <c r="A18" s="118"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="131"/>
+      <c r="D18" s="129" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="95"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="96" t="s">
+      <c r="E18" s="101"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="95"/>
+      <c r="H18" s="101"/>
       <c r="I18" s="63"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -3279,20 +3279,20 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="116"/>
-      <c r="B19" s="126" t="s">
+      <c r="A19" s="98"/>
+      <c r="B19" s="132" t="s">
         <v>379</v>
       </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="96" t="s">
+      <c r="C19" s="133"/>
+      <c r="D19" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="96" t="s">
-        <v>460</v>
-      </c>
-      <c r="H19" s="95"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="100" t="s">
+        <v>459</v>
+      </c>
+      <c r="H19" s="101"/>
       <c r="I19" s="63"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -3313,18 +3313,18 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="99" t="s">
+      <c r="A20" s="98"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="105" t="s">
         <v>371</v>
       </c>
-      <c r="E20" s="95"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="96" t="s">
+      <c r="E20" s="101"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="95"/>
+      <c r="H20" s="101"/>
       <c r="I20" s="63"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -3345,17 +3345,17 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116"/>
+      <c r="A21" s="98"/>
       <c r="B21" s="63"/>
       <c r="C21" s="57"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="103"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="108"/>
       <c r="G21" s="57"/>
-      <c r="H21" s="96" t="s">
+      <c r="H21" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="95"/>
+      <c r="I21" s="101"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -3375,17 +3375,17 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="63"/>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
-      <c r="F22" s="103"/>
+      <c r="F22" s="108"/>
       <c r="G22" s="63"/>
-      <c r="H22" s="96" t="s">
+      <c r="H22" s="100" t="s">
         <v>384</v>
       </c>
-      <c r="I22" s="95"/>
+      <c r="I22" s="101"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
@@ -3405,17 +3405,17 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
-      <c r="F23" s="103"/>
+      <c r="F23" s="108"/>
       <c r="G23" s="63"/>
-      <c r="H23" s="96" t="s">
+      <c r="H23" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="I23" s="95"/>
+      <c r="I23" s="101"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -3435,17 +3435,17 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="116"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="63"/>
       <c r="C24" s="63"/>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
-      <c r="F24" s="103"/>
+      <c r="F24" s="108"/>
       <c r="G24" s="63"/>
-      <c r="H24" s="96" t="s">
+      <c r="H24" s="100" t="s">
         <v>372</v>
       </c>
-      <c r="I24" s="95"/>
+      <c r="I24" s="101"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -3465,15 +3465,15 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="116"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="63"/>
       <c r="C25" s="63"/>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
-      <c r="F25" s="103"/>
+      <c r="F25" s="108"/>
       <c r="G25" s="63"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="95"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="101"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -3493,12 +3493,12 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="118"/>
+      <c r="A26" s="99"/>
       <c r="B26" s="63"/>
       <c r="C26" s="63"/>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
-      <c r="F26" s="104"/>
+      <c r="F26" s="109"/>
       <c r="G26" s="56"/>
       <c r="H26" s="63"/>
       <c r="I26" s="63"/>
@@ -3521,15 +3521,15 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="41" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="110"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="112"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="123"/>
       <c r="J27" s="39"/>
       <c r="K27" s="39"/>
       <c r="L27" s="39"/>
@@ -3549,7 +3549,7 @@
       <c r="Z27" s="40"/>
     </row>
     <row r="28" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="97" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="56" t="s">
@@ -3562,7 +3562,7 @@
         <v>84</v>
       </c>
       <c r="E28" s="57"/>
-      <c r="F28" s="102" t="s">
+      <c r="F28" s="94" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="56" t="s">
@@ -3593,7 +3593,7 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116"/>
+      <c r="A29" s="98"/>
       <c r="B29" s="56" t="s">
         <v>87</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="E29" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="138"/>
+      <c r="F29" s="95"/>
       <c r="G29" s="56" t="s">
         <v>18</v>
       </c>
@@ -3635,7 +3635,7 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="56" t="s">
         <v>401</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="E30" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="138"/>
+      <c r="F30" s="95"/>
       <c r="G30" s="56" t="s">
         <v>414</v>
       </c>
@@ -3677,7 +3677,7 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="56" t="s">
         <v>95</v>
       </c>
@@ -3690,7 +3690,7 @@
       <c r="E31" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="F31" s="138"/>
+      <c r="F31" s="95"/>
       <c r="G31" s="56" t="s">
         <v>28</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="116"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="56" t="s">
         <v>100</v>
       </c>
@@ -3727,12 +3727,12 @@
         <v>101</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E32" s="56" t="s">
         <v>403</v>
       </c>
-      <c r="F32" s="138"/>
+      <c r="F32" s="95"/>
       <c r="G32" s="56" t="s">
         <v>102</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="116"/>
+      <c r="A33" s="98"/>
       <c r="B33" s="56" t="s">
         <v>104</v>
       </c>
@@ -3774,7 +3774,7 @@
       <c r="E33" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="F33" s="138"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="56" t="s">
         <v>108</v>
       </c>
@@ -3803,7 +3803,7 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="116"/>
+      <c r="A34" s="98"/>
       <c r="B34" s="56"/>
       <c r="C34" s="56" t="s">
         <v>405</v>
@@ -3814,7 +3814,7 @@
       <c r="E34" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="138"/>
+      <c r="F34" s="95"/>
       <c r="G34" s="56" t="s">
         <v>113</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="116"/>
+      <c r="A35" s="98"/>
       <c r="B35" s="61" t="s">
         <v>114</v>
       </c>
@@ -3847,12 +3847,12 @@
         <v>115</v>
       </c>
       <c r="D35" s="56" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E35" s="56" t="s">
-        <v>471</v>
-      </c>
-      <c r="F35" s="138"/>
+        <v>470</v>
+      </c>
+      <c r="F35" s="95"/>
       <c r="G35" s="56" t="s">
         <v>116</v>
       </c>
@@ -3879,20 +3879,20 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="116"/>
+      <c r="A36" s="98"/>
       <c r="B36" s="61" t="s">
         <v>118</v>
       </c>
       <c r="C36" s="56" t="s">
+        <v>474</v>
+      </c>
+      <c r="D36" s="56" t="s">
         <v>475</v>
       </c>
-      <c r="D36" s="56" t="s">
+      <c r="E36" s="56" t="s">
         <v>476</v>
       </c>
-      <c r="E36" s="56" t="s">
-        <v>477</v>
-      </c>
-      <c r="F36" s="138"/>
+      <c r="F36" s="95"/>
       <c r="G36" s="56" t="s">
         <v>381</v>
       </c>
@@ -3919,12 +3919,12 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="116"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="56" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D37" s="56" t="s">
         <v>121</v>
@@ -3932,7 +3932,7 @@
       <c r="E37" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="F37" s="138"/>
+      <c r="F37" s="95"/>
       <c r="G37" s="61" t="s">
         <v>123</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="116"/>
+      <c r="A38" s="98"/>
       <c r="B38" s="57"/>
       <c r="C38" s="56" t="s">
         <v>416</v>
@@ -3970,14 +3970,14 @@
       <c r="E38" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="138"/>
+      <c r="F38" s="95"/>
       <c r="G38" s="61" t="s">
-        <v>456</v>
-      </c>
-      <c r="H38" s="96" t="s">
+        <v>455</v>
+      </c>
+      <c r="H38" s="100" t="s">
         <v>386</v>
       </c>
-      <c r="I38" s="95"/>
+      <c r="I38" s="101"/>
       <c r="J38" s="7"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -3997,9 +3997,9 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="116"/>
+      <c r="A39" s="98"/>
       <c r="B39" s="61" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C39" s="56" t="s">
         <v>365</v>
@@ -4010,14 +4010,14 @@
       <c r="E39" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="F39" s="138"/>
+      <c r="F39" s="95"/>
       <c r="G39" s="56" t="s">
-        <v>457</v>
-      </c>
-      <c r="H39" s="96" t="s">
+        <v>456</v>
+      </c>
+      <c r="H39" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="I39" s="95"/>
+      <c r="I39" s="101"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
@@ -4037,7 +4037,7 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="116"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="61" t="s">
         <v>129</v>
       </c>
@@ -4048,14 +4048,14 @@
       <c r="E40" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F40" s="138"/>
+      <c r="F40" s="95"/>
       <c r="G40" s="87" t="s">
-        <v>502</v>
-      </c>
-      <c r="H40" s="96" t="s">
+        <v>501</v>
+      </c>
+      <c r="H40" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="I40" s="95"/>
+      <c r="I40" s="101"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
@@ -4075,16 +4075,16 @@
       <c r="Z40" s="8"/>
     </row>
     <row r="41" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="116"/>
+      <c r="A41" s="98"/>
       <c r="B41" s="61" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="56"/>
       <c r="D41" s="63"/>
       <c r="E41" s="69" t="s">
-        <v>438</v>
-      </c>
-      <c r="F41" s="138"/>
+        <v>437</v>
+      </c>
+      <c r="F41" s="95"/>
       <c r="G41" s="61" t="s">
         <v>134</v>
       </c>
@@ -4109,21 +4109,21 @@
       <c r="Z41" s="8"/>
     </row>
     <row r="42" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="116"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="61" t="s">
         <v>135</v>
       </c>
       <c r="C42" s="63"/>
       <c r="D42" s="56"/>
       <c r="E42" s="63"/>
-      <c r="F42" s="138"/>
+      <c r="F42" s="95"/>
       <c r="G42" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="H42" s="96" t="s">
-        <v>452</v>
-      </c>
-      <c r="I42" s="95"/>
+      <c r="H42" s="100" t="s">
+        <v>451</v>
+      </c>
+      <c r="I42" s="101"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
@@ -4143,23 +4143,23 @@
       <c r="Z42" s="8"/>
     </row>
     <row r="43" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="116"/>
-      <c r="B43" s="96" t="s">
+      <c r="A43" s="98"/>
+      <c r="B43" s="100" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="96" t="s">
+      <c r="C43" s="101"/>
+      <c r="D43" s="100" t="s">
         <v>138</v>
       </c>
-      <c r="E43" s="95"/>
-      <c r="F43" s="138"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="95"/>
       <c r="G43" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="H43" s="96" t="s">
+      <c r="H43" s="100" t="s">
         <v>377</v>
       </c>
-      <c r="I43" s="95"/>
+      <c r="I43" s="101"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -4179,18 +4179,18 @@
       <c r="Z43" s="8"/>
     </row>
     <row r="44" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="116"/>
-      <c r="B44" s="96" t="s">
+      <c r="A44" s="98"/>
+      <c r="B44" s="100" t="s">
         <v>373</v>
       </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="96" t="s">
+      <c r="C44" s="101"/>
+      <c r="D44" s="100" t="s">
         <v>385</v>
       </c>
-      <c r="E44" s="95"/>
-      <c r="F44" s="138"/>
-      <c r="H44" s="96"/>
-      <c r="I44" s="95"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="95"/>
+      <c r="H44" s="100"/>
+      <c r="I44" s="101"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
@@ -4210,14 +4210,14 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="116"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="95"/>
-      <c r="D45" s="97" t="s">
-        <v>521</v>
-      </c>
-      <c r="E45" s="98"/>
-      <c r="F45" s="138"/>
+      <c r="A45" s="98"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="102" t="s">
+        <v>520</v>
+      </c>
+      <c r="E45" s="103"/>
+      <c r="F45" s="95"/>
       <c r="G45" s="57"/>
       <c r="H45" s="63"/>
       <c r="I45" s="63"/>
@@ -4240,16 +4240,16 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="116"/>
-      <c r="B46" s="97" t="s">
-        <v>524</v>
-      </c>
-      <c r="C46" s="98"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="138"/>
-      <c r="G46" s="99"/>
-      <c r="H46" s="95"/>
+      <c r="A46" s="98"/>
+      <c r="B46" s="102" t="s">
+        <v>523</v>
+      </c>
+      <c r="C46" s="103"/>
+      <c r="D46" s="100"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="95"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="101"/>
       <c r="I46" s="68"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
@@ -4270,22 +4270,22 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="118"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="97" t="s">
-        <v>525</v>
-      </c>
-      <c r="D47" s="98"/>
+      <c r="C47" s="102" t="s">
+        <v>524</v>
+      </c>
+      <c r="D47" s="103"/>
       <c r="E47" s="61" t="s">
-        <v>451</v>
-      </c>
-      <c r="F47" s="138"/>
-      <c r="G47" s="130" t="s">
+        <v>450</v>
+      </c>
+      <c r="F47" s="95"/>
+      <c r="G47" s="104" t="s">
         <v>141</v>
       </c>
-      <c r="H47" s="95"/>
+      <c r="H47" s="101"/>
       <c r="I47" s="71"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
@@ -4307,17 +4307,17 @@
     </row>
     <row r="48" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="94" t="s">
-        <v>450</v>
-      </c>
-      <c r="C48" s="95"/>
+      <c r="B48" s="110" t="s">
+        <v>449</v>
+      </c>
+      <c r="C48" s="101"/>
       <c r="D48" s="63"/>
       <c r="E48" s="63"/>
-      <c r="F48" s="138"/>
-      <c r="G48" s="135" t="s">
-        <v>440</v>
-      </c>
-      <c r="H48" s="136"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="116" t="s">
+        <v>439</v>
+      </c>
+      <c r="H48" s="117"/>
       <c r="I48" s="71"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
@@ -4339,15 +4339,15 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="95"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
-      <c r="F49" s="138"/>
-      <c r="G49" s="130" t="s">
+      <c r="F49" s="95"/>
+      <c r="G49" s="104" t="s">
         <v>368</v>
       </c>
-      <c r="H49" s="95"/>
+      <c r="H49" s="101"/>
       <c r="I49" s="68"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
@@ -4373,7 +4373,7 @@
       <c r="C50" s="56"/>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
-      <c r="F50" s="139"/>
+      <c r="F50" s="96"/>
       <c r="G50" s="68"/>
       <c r="H50" s="68"/>
       <c r="I50" s="68"/>
@@ -4396,15 +4396,15 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="45" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="132"/>
-      <c r="B51" s="133"/>
-      <c r="C51" s="133"/>
-      <c r="D51" s="133"/>
-      <c r="E51" s="133"/>
-      <c r="F51" s="133"/>
-      <c r="G51" s="133"/>
-      <c r="H51" s="133"/>
-      <c r="I51" s="134"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+      <c r="G51" s="113"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="114"/>
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
       <c r="L51" s="43"/>
@@ -4424,18 +4424,18 @@
       <c r="Z51" s="44"/>
     </row>
     <row r="52" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="115" t="s">
+      <c r="A52" s="97" t="s">
         <v>142</v>
       </c>
       <c r="B52" s="72"/>
       <c r="C52" s="72"/>
       <c r="D52" s="72"/>
       <c r="E52" s="63"/>
-      <c r="F52" s="119" t="s">
+      <c r="F52" s="107" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="56" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H52" s="63"/>
       <c r="I52" s="69"/>
@@ -4458,20 +4458,20 @@
       <c r="Z52" s="8"/>
     </row>
     <row r="53" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="116"/>
+      <c r="A53" s="98"/>
       <c r="B53" s="61" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C53" s="86" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D53" s="56" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="56" t="s">
-        <v>449</v>
-      </c>
-      <c r="F53" s="103"/>
+        <v>448</v>
+      </c>
+      <c r="F53" s="108"/>
       <c r="G53" s="56" t="s">
         <v>83</v>
       </c>
@@ -4500,9 +4500,9 @@
       <c r="Z53" s="8"/>
     </row>
     <row r="54" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
+      <c r="A54" s="98"/>
       <c r="B54" s="56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C54" s="56" t="s">
         <v>144</v>
@@ -4511,7 +4511,7 @@
         <v>19</v>
       </c>
       <c r="E54" s="57"/>
-      <c r="F54" s="103"/>
+      <c r="F54" s="108"/>
       <c r="G54" s="56" t="s">
         <v>88</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="116"/>
+      <c r="A55" s="98"/>
       <c r="B55" s="56" t="s">
         <v>147</v>
       </c>
@@ -4553,15 +4553,15 @@
       <c r="E55" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="F55" s="103"/>
+      <c r="F55" s="108"/>
       <c r="G55" s="56" t="s">
         <v>91</v>
       </c>
       <c r="H55" s="87" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I55" s="56" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
@@ -4582,12 +4582,12 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="116"/>
+      <c r="A56" s="98"/>
       <c r="B56" s="56" t="s">
         <v>406</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D56" s="56" t="s">
         <v>29</v>
@@ -4595,12 +4595,12 @@
       <c r="E56" s="56" t="s">
         <v>382</v>
       </c>
-      <c r="F56" s="103"/>
+      <c r="F56" s="108"/>
       <c r="G56" s="56" t="s">
         <v>150</v>
       </c>
       <c r="H56" s="56" t="s">
-        <v>420</v>
+        <v>527</v>
       </c>
       <c r="I56" s="56" t="s">
         <v>151</v>
@@ -4624,7 +4624,7 @@
       <c r="Z56" s="8"/>
     </row>
     <row r="57" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
+      <c r="A57" s="98"/>
       <c r="B57" s="56" t="s">
         <v>152</v>
       </c>
@@ -4637,7 +4637,7 @@
       <c r="E57" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="F57" s="103"/>
+      <c r="F57" s="108"/>
       <c r="G57" s="56" t="s">
         <v>155</v>
       </c>
@@ -4666,25 +4666,25 @@
       <c r="Z57" s="8"/>
     </row>
     <row r="58" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="116"/>
+      <c r="A58" s="98"/>
       <c r="B58" s="56" t="s">
         <v>156</v>
       </c>
       <c r="C58" s="56" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D58" s="56" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E58" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="F58" s="103"/>
+      <c r="F58" s="108"/>
       <c r="G58" s="56" t="s">
         <v>158</v>
       </c>
       <c r="H58" s="56" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I58" s="56" t="s">
         <v>51</v>
@@ -4708,7 +4708,7 @@
       <c r="Z58" s="8"/>
     </row>
     <row r="59" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="116"/>
+      <c r="A59" s="98"/>
       <c r="B59" s="56" t="s">
         <v>159</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="E59" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="F59" s="103"/>
+      <c r="F59" s="108"/>
       <c r="G59" s="56" t="s">
         <v>163</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>394</v>
       </c>
       <c r="I59" s="56" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -4750,7 +4750,7 @@
       <c r="Z59" s="8"/>
     </row>
     <row r="60" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="116"/>
+      <c r="A60" s="98"/>
       <c r="B60" s="56" t="s">
         <v>164</v>
       </c>
@@ -4763,12 +4763,12 @@
       <c r="E60" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="F60" s="103"/>
+      <c r="F60" s="108"/>
       <c r="G60" s="56" t="s">
         <v>168</v>
       </c>
       <c r="H60" s="56" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I60" s="74"/>
       <c r="J60" s="7"/>
@@ -4790,7 +4790,7 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
+      <c r="A61" s="98"/>
       <c r="B61" s="56" t="s">
         <v>169</v>
       </c>
@@ -4803,14 +4803,14 @@
       <c r="E61" s="56" t="s">
         <v>407</v>
       </c>
-      <c r="F61" s="103"/>
+      <c r="F61" s="108"/>
       <c r="G61" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="H61" s="94" t="s">
-        <v>491</v>
-      </c>
-      <c r="I61" s="108"/>
+      <c r="H61" s="110" t="s">
+        <v>490</v>
+      </c>
+      <c r="I61" s="115"/>
       <c r="J61" s="12"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -4830,20 +4830,20 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="116"/>
+      <c r="A62" s="98"/>
       <c r="B62" s="61" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D62" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="F62" s="103"/>
+      <c r="F62" s="108"/>
       <c r="G62" s="56"/>
-      <c r="H62" s="96"/>
-      <c r="I62" s="95"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="101"/>
       <c r="J62" s="12"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -4863,7 +4863,7 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="116"/>
+      <c r="A63" s="98"/>
       <c r="B63" s="63"/>
       <c r="C63" s="75" t="s">
         <v>174</v>
@@ -4872,13 +4872,13 @@
         <v>175</v>
       </c>
       <c r="E63" s="56" t="s">
-        <v>428</v>
-      </c>
-      <c r="F63" s="103"/>
-      <c r="G63" s="96" t="s">
+        <v>427</v>
+      </c>
+      <c r="F63" s="108"/>
+      <c r="G63" s="100" t="s">
         <v>378</v>
       </c>
-      <c r="H63" s="95"/>
+      <c r="H63" s="101"/>
       <c r="I63" s="69"/>
       <c r="J63" s="12"/>
       <c r="K63" s="7"/>
@@ -4899,22 +4899,22 @@
       <c r="Z63" s="8"/>
     </row>
     <row r="64" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="116"/>
-      <c r="B64" s="94" t="s">
-        <v>489</v>
-      </c>
-      <c r="C64" s="108"/>
+      <c r="A64" s="98"/>
+      <c r="B64" s="110" t="s">
+        <v>488</v>
+      </c>
+      <c r="C64" s="115"/>
       <c r="D64" s="56" t="s">
         <v>176</v>
       </c>
       <c r="E64" s="56" t="s">
         <v>177</v>
       </c>
-      <c r="F64" s="103"/>
-      <c r="G64" s="97" t="s">
-        <v>522</v>
-      </c>
-      <c r="H64" s="98"/>
+      <c r="F64" s="108"/>
+      <c r="G64" s="102" t="s">
+        <v>521</v>
+      </c>
+      <c r="H64" s="103"/>
       <c r="I64" s="69"/>
       <c r="J64" s="12"/>
       <c r="K64" s="7"/>
@@ -4935,20 +4935,20 @@
       <c r="Z64" s="8"/>
     </row>
     <row r="65" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="116"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="95"/>
+      <c r="A65" s="98"/>
+      <c r="B65" s="100"/>
+      <c r="C65" s="101"/>
       <c r="D65" s="56" t="s">
         <v>178</v>
       </c>
       <c r="E65" s="56" t="s">
-        <v>444</v>
-      </c>
-      <c r="F65" s="103"/>
-      <c r="G65" s="96" t="s">
-        <v>498</v>
-      </c>
-      <c r="H65" s="95"/>
+        <v>443</v>
+      </c>
+      <c r="F65" s="108"/>
+      <c r="G65" s="100" t="s">
+        <v>497</v>
+      </c>
+      <c r="H65" s="101"/>
       <c r="I65" s="69"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -4969,19 +4969,19 @@
       <c r="Z65" s="8"/>
     </row>
     <row r="66" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="116"/>
-      <c r="B66" s="96" t="s">
+      <c r="A66" s="98"/>
+      <c r="B66" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="C66" s="95"/>
+      <c r="C66" s="101"/>
       <c r="D66" s="56" t="s">
         <v>179</v>
       </c>
       <c r="E66" s="57"/>
-      <c r="F66" s="103"/>
+      <c r="F66" s="108"/>
       <c r="G66" s="57"/>
       <c r="H66" s="56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I66" s="69"/>
       <c r="J66" s="7"/>
@@ -5003,18 +5003,18 @@
       <c r="Z66" s="8"/>
     </row>
     <row r="67" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="116"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="95"/>
+      <c r="A67" s="98"/>
+      <c r="B67" s="100"/>
+      <c r="C67" s="101"/>
       <c r="D67" s="56" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E67" s="76" t="s">
         <v>396</v>
       </c>
-      <c r="F67" s="103"/>
-      <c r="G67" s="96"/>
-      <c r="H67" s="95"/>
+      <c r="F67" s="108"/>
+      <c r="G67" s="100"/>
+      <c r="H67" s="101"/>
       <c r="I67" s="69"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -5035,18 +5035,18 @@
       <c r="Z67" s="8"/>
     </row>
     <row r="68" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="116"/>
-      <c r="B68" s="96" t="s">
+      <c r="A68" s="98"/>
+      <c r="B68" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="C68" s="95"/>
-      <c r="D68" s="96" t="s">
+      <c r="C68" s="101"/>
+      <c r="D68" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="E68" s="95"/>
-      <c r="F68" s="103"/>
-      <c r="G68" s="137"/>
-      <c r="H68" s="95"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="108"/>
+      <c r="G68" s="111"/>
+      <c r="H68" s="101"/>
       <c r="I68" s="63"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
@@ -5067,18 +5067,18 @@
       <c r="Z68" s="8"/>
     </row>
     <row r="69" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="116"/>
-      <c r="B69" s="96" t="s">
+      <c r="A69" s="98"/>
+      <c r="B69" s="100" t="s">
         <v>387</v>
       </c>
-      <c r="C69" s="95"/>
-      <c r="D69" s="96" t="s">
+      <c r="C69" s="101"/>
+      <c r="D69" s="100" t="s">
         <v>388</v>
       </c>
-      <c r="E69" s="95"/>
-      <c r="F69" s="103"/>
-      <c r="G69" s="137"/>
-      <c r="H69" s="95"/>
+      <c r="E69" s="101"/>
+      <c r="F69" s="108"/>
+      <c r="G69" s="111"/>
+      <c r="H69" s="101"/>
       <c r="I69" s="63"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5099,14 +5099,14 @@
       <c r="Z69" s="8"/>
     </row>
     <row r="70" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="116"/>
+      <c r="A70" s="98"/>
       <c r="B70" s="63"/>
       <c r="C70" s="63"/>
       <c r="D70" s="63"/>
       <c r="E70" s="63"/>
-      <c r="F70" s="103"/>
-      <c r="G70" s="137"/>
-      <c r="H70" s="95"/>
+      <c r="F70" s="108"/>
+      <c r="G70" s="111"/>
+      <c r="H70" s="101"/>
       <c r="I70" s="63"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5127,17 +5127,17 @@
       <c r="Z70" s="8"/>
     </row>
     <row r="71" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="116"/>
+      <c r="A71" s="98"/>
       <c r="B71" s="63"/>
       <c r="C71" s="63"/>
       <c r="D71" s="70"/>
       <c r="E71" s="70"/>
-      <c r="F71" s="103"/>
+      <c r="F71" s="108"/>
       <c r="G71" s="77"/>
-      <c r="H71" s="96" t="s">
+      <c r="H71" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="I71" s="95"/>
+      <c r="I71" s="101"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
       <c r="L71" s="7"/>
@@ -5157,17 +5157,17 @@
       <c r="Z71" s="8"/>
     </row>
     <row r="72" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="116"/>
-      <c r="B72" s="99"/>
-      <c r="C72" s="95"/>
+      <c r="A72" s="98"/>
+      <c r="B72" s="105"/>
+      <c r="C72" s="101"/>
       <c r="D72" s="69"/>
       <c r="E72" s="69"/>
-      <c r="F72" s="103"/>
+      <c r="F72" s="108"/>
       <c r="G72" s="69"/>
-      <c r="H72" s="96" t="s">
+      <c r="H72" s="100" t="s">
         <v>183</v>
       </c>
-      <c r="I72" s="95"/>
+      <c r="I72" s="101"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
       <c r="L72" s="7"/>
@@ -5187,17 +5187,17 @@
       <c r="Z72" s="8"/>
     </row>
     <row r="73" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="116"/>
+      <c r="A73" s="98"/>
       <c r="B73" s="69"/>
       <c r="C73" s="69"/>
       <c r="D73" s="69"/>
       <c r="E73" s="69"/>
-      <c r="F73" s="103"/>
+      <c r="F73" s="108"/>
       <c r="G73" s="69"/>
-      <c r="H73" s="96" t="s">
+      <c r="H73" s="100" t="s">
         <v>390</v>
       </c>
-      <c r="I73" s="95"/>
+      <c r="I73" s="101"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
@@ -5217,12 +5217,12 @@
       <c r="Z73" s="8"/>
     </row>
     <row r="74" spans="1:26" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="116"/>
+      <c r="A74" s="98"/>
       <c r="B74" s="69"/>
       <c r="C74" s="69"/>
       <c r="D74" s="69"/>
       <c r="E74" s="69"/>
-      <c r="F74" s="103"/>
+      <c r="F74" s="108"/>
       <c r="G74" s="69"/>
       <c r="H74" s="69"/>
       <c r="I74" s="69"/>
@@ -5245,17 +5245,17 @@
       <c r="Z74" s="8"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="118"/>
+      <c r="A75" s="99"/>
       <c r="B75" s="69"/>
       <c r="C75" s="69"/>
       <c r="D75" s="69"/>
       <c r="E75" s="69"/>
-      <c r="F75" s="104"/>
+      <c r="F75" s="109"/>
       <c r="G75" s="69"/>
-      <c r="H75" s="96" t="s">
+      <c r="H75" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="I75" s="95"/>
+      <c r="I75" s="101"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
@@ -5303,7 +5303,7 @@
       <c r="Z76" s="51"/>
     </row>
     <row r="77" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="128" t="s">
+      <c r="A77" s="106" t="s">
         <v>185</v>
       </c>
       <c r="B77" s="56" t="s">
@@ -5318,7 +5318,7 @@
       <c r="E77" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F77" s="102" t="s">
+      <c r="F77" s="94" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="56" t="s">
@@ -5328,7 +5328,7 @@
         <v>82</v>
       </c>
       <c r="I77" s="56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -5349,9 +5349,9 @@
       <c r="Z77" s="8"/>
     </row>
     <row r="78" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="116"/>
+      <c r="A78" s="98"/>
       <c r="B78" s="87" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C78" s="56" t="s">
         <v>89</v>
@@ -5362,7 +5362,7 @@
       <c r="E78" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="F78" s="103"/>
+      <c r="F78" s="108"/>
       <c r="G78" s="56" t="s">
         <v>90</v>
       </c>
@@ -5391,9 +5391,9 @@
       <c r="Z78" s="8"/>
     </row>
     <row r="79" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="116"/>
+      <c r="A79" s="98"/>
       <c r="B79" s="56" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C79" s="56" t="s">
         <v>187</v>
@@ -5404,7 +5404,7 @@
       <c r="E79" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="F79" s="103"/>
+      <c r="F79" s="108"/>
       <c r="G79" s="56" t="s">
         <v>93</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>401</v>
       </c>
       <c r="I79" s="85" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -5433,7 +5433,7 @@
       <c r="Z79" s="8"/>
     </row>
     <row r="80" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="116"/>
+      <c r="A80" s="98"/>
       <c r="B80" s="56" t="s">
         <v>188</v>
       </c>
@@ -5446,7 +5446,7 @@
       <c r="E80" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="F80" s="103"/>
+      <c r="F80" s="108"/>
       <c r="G80" s="56" t="s">
         <v>98</v>
       </c>
@@ -5475,7 +5475,7 @@
       <c r="Z80" s="8"/>
     </row>
     <row r="81" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="116"/>
+      <c r="A81" s="98"/>
       <c r="B81" s="56" t="s">
         <v>191</v>
       </c>
@@ -5488,7 +5488,7 @@
       <c r="E81" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="F81" s="103"/>
+      <c r="F81" s="108"/>
       <c r="G81" s="56" t="s">
         <v>403</v>
       </c>
@@ -5512,7 +5512,7 @@
       <c r="Z81" s="8"/>
     </row>
     <row r="82" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
+      <c r="A82" s="98"/>
       <c r="B82" s="56" t="s">
         <v>194</v>
       </c>
@@ -5520,12 +5520,12 @@
         <v>195</v>
       </c>
       <c r="D82" s="56" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E82" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="F82" s="103"/>
+      <c r="F82" s="108"/>
       <c r="H82" s="61" t="s">
         <v>196</v>
       </c>
@@ -5549,12 +5549,12 @@
       <c r="Z82" s="8"/>
     </row>
     <row r="83" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="98"/>
       <c r="B83" s="56" t="s">
         <v>197</v>
       </c>
       <c r="C83" s="56" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D83" s="56" t="s">
         <v>198</v>
@@ -5562,7 +5562,7 @@
       <c r="E83" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="F83" s="103"/>
+      <c r="F83" s="108"/>
       <c r="G83" s="61" t="s">
         <v>200</v>
       </c>
@@ -5587,17 +5587,17 @@
       <c r="Z83" s="8"/>
     </row>
     <row r="84" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
+      <c r="A84" s="98"/>
       <c r="B84" s="56" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D84" s="56" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E84" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="F84" s="103"/>
+      <c r="F84" s="108"/>
       <c r="G84" s="61" t="s">
         <v>202</v>
       </c>
@@ -5624,20 +5624,20 @@
       <c r="Z84" s="8"/>
     </row>
     <row r="85" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
+      <c r="A85" s="98"/>
       <c r="B85" s="63"/>
       <c r="C85" s="56" t="s">
         <v>204</v>
       </c>
       <c r="D85" s="56" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E85" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="F85" s="103"/>
+      <c r="F85" s="108"/>
       <c r="G85" s="61" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H85" s="61" t="s">
         <v>412</v>
@@ -5662,20 +5662,20 @@
       <c r="Z85" s="8"/>
     </row>
     <row r="86" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
+      <c r="A86" s="98"/>
       <c r="B86" s="56"/>
       <c r="C86" s="56" t="s">
         <v>206</v>
       </c>
       <c r="D86" s="56" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E86" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="F86" s="103"/>
+      <c r="F86" s="108"/>
       <c r="G86" s="61" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H86" s="61" t="s">
         <v>413</v>
@@ -5700,18 +5700,18 @@
       <c r="Z86" s="8"/>
     </row>
     <row r="87" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="116"/>
-      <c r="B87" s="130" t="s">
+      <c r="A87" s="98"/>
+      <c r="B87" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="95"/>
+      <c r="C87" s="101"/>
       <c r="D87" s="56" t="s">
         <v>209</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>437</v>
-      </c>
-      <c r="F87" s="103"/>
+        <v>436</v>
+      </c>
+      <c r="F87" s="108"/>
       <c r="G87" s="61" t="s">
         <v>210</v>
       </c>
@@ -5736,25 +5736,25 @@
       <c r="Z87" s="8"/>
     </row>
     <row r="88" spans="1:26" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="116"/>
-      <c r="B88" s="130" t="s">
-        <v>441</v>
-      </c>
-      <c r="C88" s="95"/>
+      <c r="A88" s="98"/>
+      <c r="B88" s="104" t="s">
+        <v>440</v>
+      </c>
+      <c r="C88" s="101"/>
       <c r="D88" s="56" t="s">
         <v>213</v>
       </c>
       <c r="E88" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="F88" s="103"/>
+      <c r="F88" s="108"/>
       <c r="G88" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="H88" s="94" t="s">
-        <v>516</v>
-      </c>
-      <c r="I88" s="95"/>
+      <c r="H88" s="110" t="s">
+        <v>515</v>
+      </c>
+      <c r="I88" s="101"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
       <c r="L88" s="7"/>
@@ -5774,18 +5774,18 @@
       <c r="Z88" s="8"/>
     </row>
     <row r="89" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="116"/>
-      <c r="B89" s="130" t="s">
+      <c r="A89" s="98"/>
+      <c r="B89" s="104" t="s">
         <v>369</v>
       </c>
-      <c r="C89" s="95"/>
+      <c r="C89" s="101"/>
       <c r="E89" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="F89" s="103"/>
+      <c r="F89" s="108"/>
       <c r="G89" s="57"/>
-      <c r="H89" s="96"/>
-      <c r="I89" s="95"/>
+      <c r="H89" s="100"/>
+      <c r="I89" s="101"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
@@ -5805,20 +5805,20 @@
       <c r="Z89" s="8"/>
     </row>
     <row r="90" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="116"/>
-      <c r="B90" s="99"/>
-      <c r="C90" s="95"/>
+      <c r="A90" s="98"/>
+      <c r="B90" s="105"/>
+      <c r="C90" s="101"/>
       <c r="D90" s="81" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="F90" s="103"/>
-      <c r="G90" s="96" t="s">
+        <v>496</v>
+      </c>
+      <c r="F90" s="108"/>
+      <c r="G90" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="H90" s="95"/>
+      <c r="H90" s="101"/>
       <c r="I90" s="69"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
@@ -5839,18 +5839,18 @@
       <c r="Z90" s="8"/>
     </row>
     <row r="91" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="116"/>
-      <c r="B91" s="96" t="s">
+      <c r="A91" s="98"/>
+      <c r="B91" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C91" s="95"/>
+      <c r="C91" s="101"/>
       <c r="D91" s="56"/>
       <c r="E91" s="63"/>
-      <c r="F91" s="103"/>
-      <c r="G91" s="96" t="s">
+      <c r="F91" s="108"/>
+      <c r="G91" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="H91" s="95"/>
+      <c r="H91" s="101"/>
       <c r="I91" s="69"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
@@ -5871,18 +5871,18 @@
       <c r="Z91" s="8"/>
     </row>
     <row r="92" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="116"/>
-      <c r="B92" s="96" t="s">
+      <c r="A92" s="98"/>
+      <c r="B92" s="100" t="s">
         <v>218</v>
       </c>
-      <c r="C92" s="95"/>
+      <c r="C92" s="101"/>
       <c r="D92" s="79"/>
       <c r="E92" s="63"/>
-      <c r="F92" s="103"/>
-      <c r="G92" s="96" t="s">
+      <c r="F92" s="108"/>
+      <c r="G92" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="H92" s="95"/>
+      <c r="H92" s="101"/>
       <c r="I92" s="69"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
@@ -5903,20 +5903,20 @@
       <c r="Z92" s="8"/>
     </row>
     <row r="93" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="116"/>
-      <c r="B93" s="97" t="s">
-        <v>526</v>
-      </c>
-      <c r="C93" s="98"/>
-      <c r="D93" s="94" t="s">
+      <c r="A93" s="98"/>
+      <c r="B93" s="102" t="s">
+        <v>525</v>
+      </c>
+      <c r="C93" s="103"/>
+      <c r="D93" s="110" t="s">
         <v>408</v>
       </c>
-      <c r="E93" s="95"/>
-      <c r="F93" s="103"/>
-      <c r="G93" s="96" t="s">
+      <c r="E93" s="101"/>
+      <c r="F93" s="108"/>
+      <c r="G93" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="H93" s="95"/>
+      <c r="H93" s="101"/>
       <c r="I93" s="69"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
@@ -5937,17 +5937,17 @@
       <c r="Z93" s="8"/>
     </row>
     <row r="94" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="116"/>
-      <c r="B94" s="96"/>
-      <c r="C94" s="95"/>
-      <c r="D94" s="96"/>
-      <c r="E94" s="95"/>
-      <c r="F94" s="103"/>
+      <c r="A94" s="98"/>
+      <c r="B94" s="100"/>
+      <c r="C94" s="101"/>
+      <c r="D94" s="100"/>
+      <c r="E94" s="101"/>
+      <c r="F94" s="108"/>
       <c r="G94" s="63"/>
-      <c r="H94" s="96" t="s">
+      <c r="H94" s="100" t="s">
         <v>374</v>
       </c>
-      <c r="I94" s="95"/>
+      <c r="I94" s="101"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
@@ -5967,17 +5967,17 @@
       <c r="Z94" s="8"/>
     </row>
     <row r="95" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="116"/>
+      <c r="A95" s="98"/>
       <c r="B95" s="69"/>
       <c r="C95" s="56" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D95" s="69"/>
       <c r="E95" s="63"/>
-      <c r="F95" s="103"/>
+      <c r="F95" s="108"/>
       <c r="G95" s="63"/>
-      <c r="H95" s="96"/>
-      <c r="I95" s="95"/>
+      <c r="H95" s="100"/>
+      <c r="I95" s="101"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
@@ -5997,17 +5997,17 @@
       <c r="Z95" s="8"/>
     </row>
     <row r="96" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="116"/>
+      <c r="A96" s="98"/>
       <c r="B96" s="69"/>
       <c r="C96" s="69"/>
       <c r="D96" s="69"/>
       <c r="E96" s="69"/>
-      <c r="F96" s="103"/>
+      <c r="F96" s="108"/>
       <c r="G96" s="63"/>
-      <c r="H96" s="96" t="s">
-        <v>459</v>
-      </c>
-      <c r="I96" s="95"/>
+      <c r="H96" s="100" t="s">
+        <v>458</v>
+      </c>
+      <c r="I96" s="101"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
@@ -6027,15 +6027,15 @@
       <c r="Z96" s="8"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="116"/>
+      <c r="A97" s="98"/>
       <c r="B97" s="69"/>
       <c r="C97" s="69"/>
       <c r="D97" s="69"/>
       <c r="E97" s="69"/>
-      <c r="F97" s="103"/>
+      <c r="F97" s="108"/>
       <c r="G97" s="69"/>
-      <c r="H97" s="96"/>
-      <c r="I97" s="95"/>
+      <c r="H97" s="100"/>
+      <c r="I97" s="101"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
@@ -6055,12 +6055,12 @@
       <c r="Z97" s="8"/>
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="118"/>
+      <c r="A98" s="99"/>
       <c r="B98" s="69"/>
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
       <c r="E98" s="69"/>
-      <c r="F98" s="104"/>
+      <c r="F98" s="109"/>
       <c r="G98" s="82"/>
       <c r="H98" s="63"/>
       <c r="I98" s="63"/>
@@ -6111,7 +6111,7 @@
       <c r="Z99" s="44"/>
     </row>
     <row r="100" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="115" t="s">
+      <c r="A100" s="97" t="s">
         <v>221</v>
       </c>
       <c r="B100" s="56" t="s">
@@ -6126,17 +6126,17 @@
       <c r="E100" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="F100" s="102" t="s">
+      <c r="F100" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="G100" s="105" t="s">
+      <c r="G100" s="134" t="s">
         <v>224</v>
       </c>
       <c r="H100" s="56" t="s">
         <v>225</v>
       </c>
       <c r="I100" s="61" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
@@ -6157,7 +6157,7 @@
       <c r="Z100" s="8"/>
     </row>
     <row r="101" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="116"/>
+      <c r="A101" s="98"/>
       <c r="B101" s="56" t="s">
         <v>89</v>
       </c>
@@ -6170,8 +6170,8 @@
       <c r="E101" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="F101" s="103"/>
-      <c r="G101" s="103"/>
+      <c r="F101" s="108"/>
+      <c r="G101" s="108"/>
       <c r="H101" s="69" t="s">
         <v>228</v>
       </c>
@@ -6197,12 +6197,12 @@
       <c r="Z101" s="8"/>
     </row>
     <row r="102" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="116"/>
+      <c r="A102" s="98"/>
       <c r="B102" s="89" t="s">
         <v>187</v>
       </c>
       <c r="C102" s="89" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D102" s="56" t="s">
         <v>230</v>
@@ -6210,8 +6210,8 @@
       <c r="E102" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F102" s="103"/>
-      <c r="G102" s="103"/>
+      <c r="F102" s="108"/>
+      <c r="G102" s="108"/>
       <c r="I102" s="57"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
@@ -6232,21 +6232,21 @@
       <c r="Z102" s="8"/>
     </row>
     <row r="103" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="116"/>
+      <c r="A103" s="98"/>
       <c r="B103" s="89" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C103" s="89" t="s">
         <v>231</v>
       </c>
       <c r="D103" s="56" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E103" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="F103" s="103"/>
-      <c r="G103" s="103"/>
+      <c r="F103" s="108"/>
+      <c r="G103" s="108"/>
       <c r="H103" s="56" t="s">
         <v>232</v>
       </c>
@@ -6270,9 +6270,9 @@
       <c r="Z103" s="8"/>
     </row>
     <row r="104" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="116"/>
+      <c r="A104" s="98"/>
       <c r="B104" s="90" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C104" s="89" t="s">
         <v>233</v>
@@ -6280,8 +6280,8 @@
       <c r="E104" s="56" t="s">
         <v>403</v>
       </c>
-      <c r="F104" s="103"/>
-      <c r="G104" s="103"/>
+      <c r="F104" s="108"/>
+      <c r="G104" s="108"/>
       <c r="H104" s="56" t="s">
         <v>235</v>
       </c>
@@ -6305,23 +6305,23 @@
       <c r="Z104" s="8"/>
     </row>
     <row r="105" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="116"/>
+      <c r="A105" s="98"/>
       <c r="B105" s="89" t="s">
         <v>236</v>
       </c>
       <c r="C105" s="89" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D105" s="56" t="s">
         <v>237</v>
       </c>
       <c r="E105" s="56" t="s">
-        <v>421</v>
-      </c>
-      <c r="F105" s="103"/>
-      <c r="G105" s="103"/>
+        <v>420</v>
+      </c>
+      <c r="F105" s="108"/>
+      <c r="G105" s="108"/>
       <c r="H105" s="61" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I105" s="69"/>
       <c r="J105" s="7"/>
@@ -6343,7 +6343,7 @@
       <c r="Z105" s="8"/>
     </row>
     <row r="106" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="116"/>
+      <c r="A106" s="98"/>
       <c r="B106" s="89" t="s">
         <v>391</v>
       </c>
@@ -6354,10 +6354,10 @@
         <v>238</v>
       </c>
       <c r="E106" s="56" t="s">
-        <v>447</v>
-      </c>
-      <c r="F106" s="103"/>
-      <c r="G106" s="103"/>
+        <v>446</v>
+      </c>
+      <c r="F106" s="108"/>
+      <c r="G106" s="108"/>
       <c r="H106" s="57"/>
       <c r="I106" s="63"/>
       <c r="J106" s="7"/>
@@ -6379,7 +6379,7 @@
       <c r="Z106" s="8"/>
     </row>
     <row r="107" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="116"/>
+      <c r="A107" s="98"/>
       <c r="B107" s="89" t="s">
         <v>239</v>
       </c>
@@ -6387,13 +6387,13 @@
         <v>234</v>
       </c>
       <c r="D107" s="56" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E107" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="F107" s="103"/>
-      <c r="G107" s="103"/>
+      <c r="F107" s="108"/>
+      <c r="G107" s="108"/>
       <c r="H107" s="61" t="s">
         <v>366</v>
       </c>
@@ -6417,21 +6417,21 @@
       <c r="Z107" s="8"/>
     </row>
     <row r="108" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="116"/>
+      <c r="A108" s="98"/>
       <c r="B108" s="91" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C108" s="92" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D108" s="56" t="s">
         <v>241</v>
       </c>
       <c r="E108" s="56" t="s">
-        <v>482</v>
-      </c>
-      <c r="F108" s="103"/>
-      <c r="G108" s="103"/>
+        <v>481</v>
+      </c>
+      <c r="F108" s="108"/>
+      <c r="G108" s="108"/>
       <c r="H108" s="61" t="s">
         <v>242</v>
       </c>
@@ -6455,9 +6455,9 @@
       <c r="Z108" s="8"/>
     </row>
     <row r="109" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="117"/>
+      <c r="A109" s="118"/>
       <c r="B109" s="89" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C109" s="93"/>
       <c r="D109" s="60" t="s">
@@ -6466,8 +6466,8 @@
       <c r="E109" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="F109" s="103"/>
-      <c r="G109" s="103"/>
+      <c r="F109" s="108"/>
+      <c r="G109" s="108"/>
       <c r="H109" s="61" t="s">
         <v>245</v>
       </c>
@@ -6491,23 +6491,23 @@
       <c r="Z109" s="8"/>
     </row>
     <row r="110" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="116"/>
-      <c r="B110" s="106" t="s">
+      <c r="A110" s="98"/>
+      <c r="B110" s="135" t="s">
         <v>409</v>
       </c>
-      <c r="C110" s="107"/>
+      <c r="C110" s="136"/>
       <c r="D110" s="56" t="s">
         <v>246</v>
       </c>
       <c r="E110" s="56" t="s">
-        <v>435</v>
-      </c>
-      <c r="F110" s="103"/>
-      <c r="G110" s="103"/>
-      <c r="H110" s="94" t="s">
-        <v>458</v>
-      </c>
-      <c r="I110" s="95"/>
+        <v>434</v>
+      </c>
+      <c r="F110" s="108"/>
+      <c r="G110" s="108"/>
+      <c r="H110" s="110" t="s">
+        <v>457</v>
+      </c>
+      <c r="I110" s="101"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
       <c r="L110" s="7"/>
@@ -6527,23 +6527,23 @@
       <c r="Z110" s="8"/>
     </row>
     <row r="111" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="116"/>
-      <c r="B111" s="97" t="s">
-        <v>527</v>
-      </c>
-      <c r="C111" s="98"/>
+      <c r="A111" s="98"/>
+      <c r="B111" s="102" t="s">
+        <v>526</v>
+      </c>
+      <c r="C111" s="103"/>
       <c r="D111" s="87" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E111" s="56" t="s">
-        <v>427</v>
-      </c>
-      <c r="F111" s="103"/>
-      <c r="G111" s="103"/>
-      <c r="H111" s="94" t="s">
-        <v>494</v>
-      </c>
-      <c r="I111" s="95"/>
+        <v>426</v>
+      </c>
+      <c r="F111" s="108"/>
+      <c r="G111" s="108"/>
+      <c r="H111" s="110" t="s">
+        <v>493</v>
+      </c>
+      <c r="I111" s="101"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
       <c r="L111" s="7"/>
@@ -6563,21 +6563,21 @@
       <c r="Z111" s="8"/>
     </row>
     <row r="112" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="116"/>
-      <c r="B112" s="100"/>
-      <c r="C112" s="101"/>
+      <c r="A112" s="98"/>
+      <c r="B112" s="138"/>
+      <c r="C112" s="139"/>
       <c r="D112" s="56" t="s">
         <v>247</v>
       </c>
       <c r="E112" s="56" t="s">
-        <v>442</v>
-      </c>
-      <c r="F112" s="103"/>
-      <c r="G112" s="103"/>
-      <c r="H112" s="94" t="s">
-        <v>517</v>
-      </c>
-      <c r="I112" s="95"/>
+        <v>441</v>
+      </c>
+      <c r="F112" s="108"/>
+      <c r="G112" s="108"/>
+      <c r="H112" s="110" t="s">
+        <v>516</v>
+      </c>
+      <c r="I112" s="101"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
       <c r="L112" s="7"/>
@@ -6597,21 +6597,21 @@
       <c r="Z112" s="8"/>
     </row>
     <row r="113" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="116"/>
-      <c r="B113" s="96" t="s">
+      <c r="A113" s="98"/>
+      <c r="B113" s="100" t="s">
         <v>375</v>
       </c>
-      <c r="C113" s="95"/>
+      <c r="C113" s="101"/>
       <c r="D113" s="56" t="s">
         <v>367</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F113" s="103"/>
-      <c r="G113" s="103"/>
-      <c r="H113" s="96"/>
-      <c r="I113" s="95"/>
+        <v>495</v>
+      </c>
+      <c r="F113" s="108"/>
+      <c r="G113" s="108"/>
+      <c r="H113" s="100"/>
+      <c r="I113" s="101"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
       <c r="L113" s="7"/>
@@ -6631,21 +6631,21 @@
       <c r="Z113" s="8"/>
     </row>
     <row r="114" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="116"/>
-      <c r="B114" s="96"/>
-      <c r="C114" s="95"/>
+      <c r="A114" s="98"/>
+      <c r="B114" s="100"/>
+      <c r="C114" s="101"/>
       <c r="D114" s="56" t="s">
         <v>248</v>
       </c>
       <c r="E114" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="F114" s="103"/>
-      <c r="G114" s="103"/>
-      <c r="H114" s="97" t="s">
-        <v>523</v>
-      </c>
-      <c r="I114" s="98"/>
+      <c r="F114" s="108"/>
+      <c r="G114" s="108"/>
+      <c r="H114" s="102" t="s">
+        <v>522</v>
+      </c>
+      <c r="I114" s="103"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
       <c r="L114" s="7"/>
@@ -6665,19 +6665,19 @@
       <c r="Z114" s="8"/>
     </row>
     <row r="115" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="116"/>
-      <c r="B115" s="96" t="s">
+      <c r="A115" s="98"/>
+      <c r="B115" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="C115" s="95"/>
+      <c r="C115" s="101"/>
       <c r="D115" s="83"/>
       <c r="E115" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="F115" s="103"/>
-      <c r="G115" s="103"/>
-      <c r="H115" s="96"/>
-      <c r="I115" s="95"/>
+      <c r="F115" s="108"/>
+      <c r="G115" s="108"/>
+      <c r="H115" s="100"/>
+      <c r="I115" s="101"/>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
       <c r="L115" s="7"/>
@@ -6697,19 +6697,19 @@
       <c r="Z115" s="8"/>
     </row>
     <row r="116" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="116"/>
-      <c r="B116" s="96" t="s">
+      <c r="A116" s="98"/>
+      <c r="B116" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="C116" s="95"/>
+      <c r="C116" s="101"/>
       <c r="D116" s="79"/>
       <c r="E116" s="63"/>
-      <c r="F116" s="103"/>
-      <c r="G116" s="103"/>
-      <c r="H116" s="96" t="s">
+      <c r="F116" s="108"/>
+      <c r="G116" s="108"/>
+      <c r="H116" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="I116" s="95"/>
+      <c r="I116" s="101"/>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
       <c r="L116" s="7"/>
@@ -6729,17 +6729,17 @@
       <c r="Z116" s="8"/>
     </row>
     <row r="117" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="116"/>
-      <c r="B117" s="96" t="s">
+      <c r="A117" s="98"/>
+      <c r="B117" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="C117" s="95"/>
+      <c r="C117" s="101"/>
       <c r="D117" s="63"/>
       <c r="E117" s="69"/>
-      <c r="F117" s="103"/>
-      <c r="G117" s="103"/>
-      <c r="H117" s="96"/>
-      <c r="I117" s="95"/>
+      <c r="F117" s="108"/>
+      <c r="G117" s="108"/>
+      <c r="H117" s="100"/>
+      <c r="I117" s="101"/>
       <c r="J117" s="9"/>
       <c r="K117" s="9"/>
       <c r="L117" s="7"/>
@@ -6759,17 +6759,17 @@
       <c r="Z117" s="8"/>
     </row>
     <row r="118" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="116"/>
-      <c r="B118" s="99"/>
-      <c r="C118" s="95"/>
+      <c r="A118" s="98"/>
+      <c r="B118" s="105"/>
+      <c r="C118" s="101"/>
       <c r="D118" s="63"/>
       <c r="E118" s="69"/>
-      <c r="F118" s="103"/>
-      <c r="G118" s="103"/>
-      <c r="H118" s="96" t="s">
+      <c r="F118" s="108"/>
+      <c r="G118" s="108"/>
+      <c r="H118" s="100" t="s">
         <v>254</v>
       </c>
-      <c r="I118" s="95"/>
+      <c r="I118" s="101"/>
       <c r="J118" s="9"/>
       <c r="K118" s="9"/>
       <c r="L118" s="7"/>
@@ -6789,18 +6789,18 @@
       <c r="Z118" s="8"/>
     </row>
     <row r="119" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="116"/>
-      <c r="C119" s="94" t="s">
-        <v>493</v>
-      </c>
-      <c r="D119" s="95"/>
+      <c r="A119" s="98"/>
+      <c r="C119" s="110" t="s">
+        <v>492</v>
+      </c>
+      <c r="D119" s="101"/>
       <c r="E119" s="69"/>
-      <c r="F119" s="103"/>
-      <c r="G119" s="104"/>
-      <c r="H119" s="96" t="s">
+      <c r="F119" s="108"/>
+      <c r="G119" s="109"/>
+      <c r="H119" s="100" t="s">
         <v>255</v>
       </c>
-      <c r="I119" s="95"/>
+      <c r="I119" s="101"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
       <c r="L119" s="7"/>
@@ -6820,16 +6820,16 @@
       <c r="Z119" s="8"/>
     </row>
     <row r="120" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="118"/>
+      <c r="A120" s="99"/>
       <c r="B120" s="69"/>
-      <c r="C120" s="96"/>
-      <c r="D120" s="95"/>
+      <c r="C120" s="100"/>
+      <c r="D120" s="101"/>
       <c r="E120" s="69"/>
-      <c r="F120" s="104"/>
-      <c r="G120" s="96" t="s">
+      <c r="F120" s="109"/>
+      <c r="G120" s="100" t="s">
         <v>256</v>
       </c>
-      <c r="H120" s="109"/>
+      <c r="H120" s="137"/>
       <c r="I120" s="71"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
@@ -6854,10 +6854,10 @@
       <c r="B121" s="11"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
-      <c r="E121" s="130" t="s">
-        <v>519</v>
-      </c>
-      <c r="F121" s="131"/>
+      <c r="E121" s="104" t="s">
+        <v>518</v>
+      </c>
+      <c r="F121" s="120"/>
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
       <c r="I121" s="11"/>
@@ -6908,7 +6908,7 @@
       <c r="Z122" s="44"/>
     </row>
     <row r="123" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="115" t="s">
+      <c r="A123" s="97" t="s">
         <v>257</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -6918,9 +6918,9 @@
         <v>259</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="F123" s="128" t="s">
+        <v>467</v>
+      </c>
+      <c r="F123" s="106" t="s">
         <v>13</v>
       </c>
       <c r="G123" s="11"/>
@@ -6945,9 +6945,9 @@
       <c r="Z123" s="8"/>
     </row>
     <row r="124" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="116"/>
+      <c r="A124" s="98"/>
       <c r="B124" s="56" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C124" s="42" t="s">
         <v>227</v>
@@ -6955,7 +6955,7 @@
       <c r="E124" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="F124" s="116"/>
+      <c r="F124" s="98"/>
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
       <c r="I124" s="16"/>
@@ -6978,14 +6978,14 @@
       <c r="Z124" s="8"/>
     </row>
     <row r="125" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="116"/>
+      <c r="A125" s="98"/>
       <c r="B125" s="69"/>
       <c r="C125" s="57"/>
       <c r="D125" s="56" t="s">
         <v>261</v>
       </c>
       <c r="E125" s="57"/>
-      <c r="F125" s="116"/>
+      <c r="F125" s="98"/>
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
       <c r="I125" s="16"/>
@@ -7008,16 +7008,16 @@
       <c r="Z125" s="8"/>
     </row>
     <row r="126" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="116"/>
+      <c r="A126" s="98"/>
       <c r="B126" s="69" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C126" s="56" t="s">
         <v>234</v>
       </c>
       <c r="D126" s="57"/>
       <c r="E126" s="63"/>
-      <c r="F126" s="116"/>
+      <c r="F126" s="98"/>
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
       <c r="I126" s="15"/>
@@ -7040,7 +7040,7 @@
       <c r="Z126" s="8"/>
     </row>
     <row r="127" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="116"/>
+      <c r="A127" s="98"/>
       <c r="B127" s="69"/>
       <c r="C127" s="56" t="s">
         <v>237</v>
@@ -7049,7 +7049,7 @@
         <v>264</v>
       </c>
       <c r="E127" s="63"/>
-      <c r="F127" s="116"/>
+      <c r="F127" s="98"/>
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
       <c r="I127" s="15"/>
@@ -7072,12 +7072,12 @@
       <c r="Z127" s="8"/>
     </row>
     <row r="128" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="116"/>
+      <c r="A128" s="98"/>
       <c r="B128" s="69"/>
       <c r="C128" s="57"/>
       <c r="D128" s="62"/>
       <c r="E128" s="66"/>
-      <c r="F128" s="116"/>
+      <c r="F128" s="98"/>
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
       <c r="I128" s="11"/>
@@ -7100,14 +7100,14 @@
       <c r="Z128" s="8"/>
     </row>
     <row r="129" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="116"/>
+      <c r="A129" s="98"/>
       <c r="B129" s="56"/>
       <c r="C129" s="81" t="s">
         <v>263</v>
       </c>
       <c r="D129" s="62"/>
       <c r="E129" s="84"/>
-      <c r="F129" s="116"/>
+      <c r="F129" s="98"/>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
       <c r="I129" s="11"/>
@@ -7130,16 +7130,16 @@
       <c r="Z129" s="8"/>
     </row>
     <row r="130" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="116"/>
-      <c r="B130" s="96" t="s">
+      <c r="A130" s="98"/>
+      <c r="B130" s="100" t="s">
         <v>410</v>
       </c>
-      <c r="C130" s="95"/>
-      <c r="D130" s="129" t="s">
-        <v>495</v>
-      </c>
-      <c r="E130" s="95"/>
-      <c r="F130" s="116"/>
+      <c r="C130" s="101"/>
+      <c r="D130" s="119" t="s">
+        <v>494</v>
+      </c>
+      <c r="E130" s="101"/>
+      <c r="F130" s="98"/>
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
       <c r="I130" s="11"/>
@@ -7162,12 +7162,12 @@
       <c r="Z130" s="8"/>
     </row>
     <row r="131" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="116"/>
-      <c r="B131" s="96"/>
-      <c r="C131" s="95"/>
-      <c r="D131" s="96"/>
-      <c r="E131" s="95"/>
-      <c r="F131" s="116"/>
+      <c r="A131" s="98"/>
+      <c r="B131" s="100"/>
+      <c r="C131" s="101"/>
+      <c r="D131" s="100"/>
+      <c r="E131" s="101"/>
+      <c r="F131" s="98"/>
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
       <c r="I131" s="11"/>
@@ -7190,16 +7190,16 @@
       <c r="Z131" s="8"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="116"/>
-      <c r="B132" s="96" t="s">
+      <c r="A132" s="98"/>
+      <c r="B132" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="C132" s="95"/>
-      <c r="D132" s="96" t="s">
+      <c r="C132" s="101"/>
+      <c r="D132" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="E132" s="95"/>
-      <c r="F132" s="116"/>
+      <c r="E132" s="101"/>
+      <c r="F132" s="98"/>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
       <c r="I132" s="11"/>
@@ -7222,16 +7222,16 @@
       <c r="Z132" s="8"/>
     </row>
     <row r="133" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="116"/>
-      <c r="B133" s="96" t="s">
+      <c r="A133" s="98"/>
+      <c r="B133" s="100" t="s">
         <v>267</v>
       </c>
-      <c r="C133" s="95"/>
-      <c r="D133" s="96" t="s">
+      <c r="C133" s="101"/>
+      <c r="D133" s="100" t="s">
         <v>393</v>
       </c>
-      <c r="E133" s="95"/>
-      <c r="F133" s="116"/>
+      <c r="E133" s="101"/>
+      <c r="F133" s="98"/>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
@@ -7254,16 +7254,16 @@
       <c r="Z133" s="8"/>
     </row>
     <row r="134" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="116"/>
-      <c r="B134" s="96" t="s">
+      <c r="A134" s="98"/>
+      <c r="B134" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="C134" s="95"/>
-      <c r="D134" s="96" t="s">
+      <c r="C134" s="101"/>
+      <c r="D134" s="100" t="s">
         <v>269</v>
       </c>
-      <c r="E134" s="95"/>
-      <c r="F134" s="118"/>
+      <c r="E134" s="101"/>
+      <c r="F134" s="99"/>
       <c r="G134" s="15"/>
       <c r="H134" s="11"/>
       <c r="I134" s="11"/>
@@ -7286,11 +7286,11 @@
       <c r="Z134" s="8"/>
     </row>
     <row r="135" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="116"/>
-      <c r="B135" s="96" t="s">
-        <v>499</v>
-      </c>
-      <c r="C135" s="95"/>
+      <c r="A135" s="98"/>
+      <c r="B135" s="100" t="s">
+        <v>498</v>
+      </c>
+      <c r="C135" s="101"/>
       <c r="D135" s="70"/>
       <c r="E135" s="70"/>
       <c r="F135" s="10"/>
@@ -7316,9 +7316,9 @@
       <c r="Z135" s="8"/>
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="118"/>
-      <c r="B136" s="94"/>
-      <c r="C136" s="108"/>
+      <c r="A136" s="99"/>
+      <c r="B136" s="110"/>
+      <c r="C136" s="115"/>
       <c r="D136" s="11"/>
       <c r="E136" s="15"/>
       <c r="F136" s="13"/>
@@ -7344,15 +7344,15 @@
       <c r="Z136" s="8"/>
     </row>
     <row r="137" spans="1:26" s="45" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="132"/>
-      <c r="B137" s="133"/>
-      <c r="C137" s="133"/>
-      <c r="D137" s="133"/>
-      <c r="E137" s="133"/>
-      <c r="F137" s="133"/>
-      <c r="G137" s="133"/>
-      <c r="H137" s="133"/>
-      <c r="I137" s="134"/>
+      <c r="A137" s="112"/>
+      <c r="B137" s="113"/>
+      <c r="C137" s="113"/>
+      <c r="D137" s="113"/>
+      <c r="E137" s="113"/>
+      <c r="F137" s="113"/>
+      <c r="G137" s="113"/>
+      <c r="H137" s="113"/>
+      <c r="I137" s="114"/>
       <c r="J137" s="44"/>
       <c r="K137" s="43"/>
       <c r="L137" s="43"/>
@@ -31735,42 +31735,77 @@
     </row>
   </sheetData>
   <mergeCells count="131">
-    <mergeCell ref="F28:F50"/>
-    <mergeCell ref="A28:A47"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A52:A75"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="A77:A98"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="F52:F75"/>
-    <mergeCell ref="F77:F98"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F100:F120"/>
+    <mergeCell ref="G100:G119"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:A26"/>
+    <mergeCell ref="F3:F26"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A100:A120"/>
+    <mergeCell ref="A123:A136"/>
+    <mergeCell ref="F123:F134"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="E121:F121"/>
     <mergeCell ref="A137:I137"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
@@ -31795,77 +31830,42 @@
     <mergeCell ref="G63:H63"/>
     <mergeCell ref="G64:H64"/>
     <mergeCell ref="H94:I94"/>
-    <mergeCell ref="A100:A120"/>
-    <mergeCell ref="A123:A136"/>
-    <mergeCell ref="F123:F134"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:A26"/>
-    <mergeCell ref="F3:F26"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="F100:F120"/>
-    <mergeCell ref="G100:G119"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="F52:F75"/>
+    <mergeCell ref="F77:F98"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="A77:A98"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="F28:F50"/>
+    <mergeCell ref="A28:A47"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A52:A75"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.35433070866141736" top="0.74803149606299213" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>